<commit_message>
Order History Session Storage
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -664,9 +664,125 @@
         <v>Chicken Burger (x3), Mango Lassi (x1)</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45686.22928240741</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>790</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45672.22928240741</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Reevan</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Oreo Shake (x2), Vanilla Shake (x1), Mango Lassi (x4)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45658.22928240741</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Notsla Daniel</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>345</v>
+      </c>
+      <c r="F12">
+        <v>2.3</v>
+      </c>
+      <c r="G12">
+        <v>1.2</v>
+      </c>
+      <c r="H12">
+        <v>3.5</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Chicken Cheese Burger (x5)</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45647.22928240741</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>895</v>
+      </c>
+      <c r="F13">
+        <v>3.9</v>
+      </c>
+      <c r="G13">
+        <v>3.2</v>
+      </c>
+      <c r="H13">
+        <v>7.1</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Chicken Cheese Pops (x3)</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Settings in ui.js is split into multiple else-ifs
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,31 +434,31 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>45693.22928240741</v>
       </c>
       <c r="C2" t="str">
-        <v>Reevan</v>
+        <v>Karthik</v>
       </c>
       <c r="D2">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>450</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I2" t="str">
-        <v>Mango Lassi (x9)</v>
+        <v>Strawberry Shake (x3)</v>
       </c>
     </row>
     <row r="3">
@@ -492,297 +492,65 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>45693.22928240741</v>
+        <v>45686.22928240741</v>
       </c>
       <c r="C4" t="str">
-        <v>Reevan</v>
+        <v>Karthik</v>
       </c>
       <c r="D4">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>790</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I4" t="str">
-        <v>Veg Cheese Pops (x1)</v>
+        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>45693.22928240741</v>
+        <v>45672.22928240741</v>
       </c>
       <c r="C5" t="str">
-        <v>Karthik</v>
+        <v>Reevan</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I5" t="str">
-        <v>Strawberry Shake (x3)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45692.22928240741</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>870</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Chicken Wrap (x9)</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45692.22928240741</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Notsla Daniel</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>800</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <v>11</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Butterscotch Lassi (x8)</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45692.22928240741</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>900</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8">
-        <v>11</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Chicken Burger (x3), Butterscotch Lassi (x7)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45687.22928240741</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>130</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Chicken Burger (x3), Mango Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45686.22928240741</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Karthik</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>790</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>15</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45672.22928240741</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Reevan</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>500</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Oreo Shake (x2), Vanilla Shake (x1), Mango Lassi (x4)</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45658.22928240741</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Notsla Daniel</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>345</v>
-      </c>
-      <c r="F12">
-        <v>2.3</v>
-      </c>
-      <c r="G12">
-        <v>1.2</v>
-      </c>
-      <c r="H12">
-        <v>3.5</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Chicken Cheese Burger (x5)</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45647.22928240741</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Karthik</v>
-      </c>
-      <c r="D13">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>895</v>
-      </c>
-      <c r="F13">
-        <v>3.9</v>
-      </c>
-      <c r="G13">
-        <v>3.2</v>
-      </c>
-      <c r="H13">
-        <v>7.1</v>
-      </c>
-      <c r="I13" t="str">
-        <v>Chicken Cheese Pops (x3)</v>
+        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Vanilla Shake (x1), Oreo Shake (x2), Mango Lassi (x4)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJOR CHANGES TO SAVE AND PRINT
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,31 +434,31 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>45693.22928240741</v>
       </c>
       <c r="C2" t="str">
-        <v>Karthik</v>
+        <v>Reevan</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E2">
-        <v>450</v>
+        <v>50</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="I2" t="str">
-        <v>Strawberry Shake (x3)</v>
+        <v>Mango Lassi (x9)</v>
       </c>
     </row>
     <row r="3">
@@ -492,65 +492,181 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Reevan</v>
+      </c>
+      <c r="D4">
+        <v>111</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>45686.22928240741</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Karthik</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>790</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>15</v>
-      </c>
       <c r="I4" t="str">
-        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
+        <v>Veg Cheese Pops (x1)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>450</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Strawberry Shake (x3)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>870</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Chicken Wrap (x9)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Notsla Daniel</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>800</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Butterscotch Lassi (x8)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>900</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Chicken Burger (x3), Butterscotch Lassi (x7)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45687.22928240741</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>130</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>45672.22928240741</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Reevan</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>500</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Vanilla Shake (x1), Oreo Shake (x2), Mango Lassi (x4)</v>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Chicken Burger (x3), Mango Lassi (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Category Wise table now has deletion option from context menu
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,244 +429,847 @@
         <v>Tax (₹)</v>
       </c>
       <c r="I1" t="str">
+        <v>Reason</v>
+      </c>
+      <c r="J1" t="str">
         <v>Food Items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1">
-        <v>45693.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C2" t="str">
-        <v>Reevan</v>
+        <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="I2" t="str">
-        <v>Mango Lassi (x9)</v>
+        <v>s</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Lime Juice (x2)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
-        <v>45693.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C3" t="str">
-        <v>Karthik</v>
+        <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I3" t="str">
-        <v>Vanilla Shake (x4)</v>
+        <v>dsf</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Mint Lime (x2), Lime Juice (x3), Watermelon Juice (x2), Weed (x2)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
-        <v>45693.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C4" t="str">
-        <v>Reevan</v>
+        <v>Ajay Francis Anchan</v>
       </c>
       <c r="D4">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="I4" t="str">
-        <v>Veg Cheese Pops (x1)</v>
+        <v>asdsd</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Chicken Cheese Burger (x1), 8PM Coffee (x2)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
-        <v>45693.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C5" t="str">
-        <v>Karthik</v>
+        <v>Ajay Francis Anchan</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>450</v>
+        <v>200</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>2.6</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>2.6</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>5.2</v>
       </c>
       <c r="I5" t="str">
-        <v>Strawberry Shake (x3)</v>
+        <v>dsgsgd</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Vanilla Shake (x2), Chicken Borgir (x2)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
-        <v>45692.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C6" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>870</v>
+        <v>180</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="I6" t="str">
-        <v>Chicken Wrap (x9)</v>
+        <v>ygug</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Chicken Borgir (x2), Chicken Cheese Burger (x1)</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1">
-        <v>45692.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C7" t="str">
-        <v>Notsla Daniel</v>
+        <v>Ajay Francis Anchan</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>800</v>
+        <v>240</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="G7">
-        <v>36</v>
+        <v>3.6</v>
       </c>
       <c r="H7">
-        <v>11</v>
+        <v>7.2</v>
       </c>
       <c r="I7" t="str">
-        <v>Butterscotch Lassi (x8)</v>
+        <v>dsfs</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Chicken Borgir (x2), Chicken Cheese Burger (x2)</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>45692.22928240741</v>
+        <v>45697.22928240741</v>
       </c>
       <c r="C8" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>900</v>
+        <v>130</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>1.43</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>1.43</v>
       </c>
       <c r="H8">
-        <v>11</v>
+        <v>2.85</v>
       </c>
       <c r="I8" t="str">
-        <v>Chicken Burger (x3), Butterscotch Lassi (x7)</v>
+        <v>y</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Oreo Shake (x1), Strawberry Lassi (x1), Vanilla Shake (x1)</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>0.8</v>
+      </c>
+      <c r="G9">
+        <v>0.8</v>
+      </c>
+      <c r="H9">
+        <v>1.6</v>
+      </c>
+      <c r="I9" t="str">
+        <v>hard coffee hard cock</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Hard Rock Coffee (x2)</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>360</v>
+      </c>
+      <c r="F10">
+        <v>5.55</v>
+      </c>
+      <c r="G10">
+        <v>5.55</v>
+      </c>
+      <c r="H10">
+        <v>11.1</v>
+      </c>
+      <c r="I10" t="str">
+        <v>ajsldj</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Chicken Cheese Pops (x1), Veg Cheese Pops (x1), Chicken Borgir (x2), Butterscotch Lassi (x1), Strawberry Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1615</v>
+      </c>
+      <c r="F11">
+        <v>19.6</v>
+      </c>
+      <c r="G11">
+        <v>20.35</v>
+      </c>
+      <c r="H11">
+        <v>39.05</v>
+      </c>
+      <c r="I11" t="str">
+        <v>sdf</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Chicken Borgir (x3), Mango Lassi (x1), Vanilla Shake (x2), Butterscotch Lassi (x1), Chicken Wrap (x1), Veg Wrap (x1), Banana Shake (x1), Black Currant Shake (x1), Strawberry Shake (x1), Chocolate Shake (x1), 8PM Coffee (x1), Coffee Italia (x1), Lime Juice (x2), Watermelon Juice (x2), Peri Peri Fries (x1), Hard Rock Coffee (x1), Chicken Momos (x1), Pomogranate Juice (x2), Strawberry Lassi (x1), Chicken Cheese Burger (x3), Oreo Shake (x1), Weed (x2)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1715</v>
+      </c>
+      <c r="F12">
+        <v>20.6</v>
+      </c>
+      <c r="G12">
+        <v>21.35</v>
+      </c>
+      <c r="H12">
+        <v>41.05</v>
+      </c>
+      <c r="I12" t="str">
+        <v>bnfj</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Chicken Borgir (x3), Chicken Cheese Burger (x3), Vanilla Shake (x2), Butterscotch Lassi (x1), Chicken Wrap (x1), Veg Wrap (x1), Banana Shake (x1), Black Currant Shake (x1), Strawberry Shake (x1), Chocolate Shake (x1), Hard Rock Coffee (x1), 8PM Coffee (x1), Coffee Italia (x1), Belgian Coffee (x1), Lime Juice (x2), Mint Lime (x2), Watermelon Juice (x2), Peri Peri Fries (x1), Chicken Momos (x1), Pomogranate Juice (x2), Weed (x2), Mango Lassi (x1), Strawberry Lassi (x1), Oreo Shake (x1)</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
+      <c r="E13">
+        <v>1795</v>
+      </c>
+      <c r="F13">
+        <v>23.8</v>
+      </c>
+      <c r="G13">
+        <v>24.55</v>
+      </c>
+      <c r="H13">
+        <v>47.69</v>
+      </c>
+      <c r="I13" t="str">
+        <v>kjhk</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Oreo Shake (x1), Mango Lassi (x1), Strawberry Lassi (x1), Chicken Borgir (x3), Chicken Wrap (x1), Veg Wrap (x1), Banana Shake (x1), Black Currant Shake (x1), Strawberry Shake (x1), Chocolate Shake (x1), 8PM Coffee (x1), Hard Rock Coffee (x1), Coffee Italia (x1), Belgian Coffee (x1), Lime Juice (x2), Mint Lime (x2), Watermelon Juice (x2), Peri Peri Fries (x1), Chicken Momos (x1), Veg Momos (x1), Pomogranate Juice (x2), Vanilla Shake (x2), Weed (x2), Chicken Cheese Burger (x3), Butterscotch Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45697.22928240741</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>840</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>18</v>
+      </c>
+      <c r="I14" t="str">
+        <v>fuck</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Vanilla Shake (x4), Coffee Italia (x5), Butterscotch Lassi (x2), Hard Rock Coffee (x3), 8PM Coffee (x6)</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45696.22928240741</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>360</v>
+      </c>
+      <c r="F15">
+        <v>4.1</v>
+      </c>
+      <c r="G15">
+        <v>4.1</v>
+      </c>
+      <c r="H15">
+        <v>8.2</v>
+      </c>
+      <c r="I15" t="str">
+        <v>ug</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Vanilla Shake (x4), Oreo Shake (x4)</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45696.22928240741</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>360</v>
+      </c>
+      <c r="F16">
+        <v>4.1</v>
+      </c>
+      <c r="G16">
+        <v>4.1</v>
+      </c>
+      <c r="H16">
+        <v>8.2</v>
+      </c>
+      <c r="I16" t="str">
+        <v>I hate my life</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Oreo Shake (x4), Vanilla Shake (x4)</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Reevan</v>
+      </c>
+      <c r="D17">
+        <v>121</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="str">
+        <v>lkj</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Mango Lassi (x9)</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>450</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18" t="str">
+        <v>skibidi</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Vanilla Shake (x4)</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Reevan</v>
+      </c>
+      <c r="D19">
+        <v>111</v>
+      </c>
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19" t="str">
+        <v>gimme mony</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Veg Cheese Pops (x1)</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45693.22928240741</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>450</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+      <c r="I20" t="str">
+        <v>I hate the number 10</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Strawberry Shake (x3)</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>254</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D21">
+        <v>909</v>
+      </c>
+      <c r="E21">
+        <v>565</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Placement Department ran out of money</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Butterscotch Lassi (x2), Chicken Wrap (x6)</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>870</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <v>kjlkj</v>
+      </c>
+      <c r="J22" t="str">
+        <v>Chicken Wrap (x9)</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C23" t="str">
+        <v>notslan Daniel</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>800</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>36</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23" t="str">
+        <v>ijlj</v>
+      </c>
+      <c r="J23" t="str">
+        <v>Butterscotch Lassi (x8)</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45692.22928240741</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>900</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>11</v>
+      </c>
+      <c r="I24" t="str">
+        <v>srcdf</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Chicken Borgir (x3), Butterscotch Lassi (x7)</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>244</v>
+      </c>
+      <c r="B25" s="1">
         <v>45687.22928240741</v>
       </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
+      <c r="C25" t="str">
+        <v>notslan Daniel</v>
+      </c>
+      <c r="D25">
+        <v>849</v>
+      </c>
+      <c r="E25">
+        <v>65</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25" t="str">
+        <v>Vegetarian got meat in the mouth</v>
+      </c>
+      <c r="J25" t="str">
+        <v>Black Currant Shake (x4), Chicken Cheese Burger (x1)</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="B26" s="1">
+        <v>45687.22928240741</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>130</v>
       </c>
-      <c r="F9">
+      <c r="F26">
         <v>2</v>
       </c>
-      <c r="G9">
+      <c r="G26">
         <v>3</v>
       </c>
-      <c r="H9">
+      <c r="H26">
         <v>5</v>
       </c>
-      <c r="I9" t="str">
-        <v>Chicken Burger (x3), Mango Lassi (x1)</v>
+      <c r="I26" t="str">
+        <v>dgcg</v>
+      </c>
+      <c r="J26" t="str">
+        <v>Chicken Borgir (x3), Mango Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45686.22928240741</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Karthik</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>790</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27" t="str">
+        <v>kjjjk</v>
+      </c>
+      <c r="J27" t="str">
+        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clear History implemented successfully in Deleted Orders Table and session storage updation
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,14 +398,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Bill No ▲</v>
+        <v>Bill No</v>
       </c>
       <c r="B1" t="str">
         <v>Date</v>
@@ -429,70 +429,47 @@
         <v>Tax (₹)</v>
       </c>
       <c r="I1" t="str">
+        <v>Reason</v>
+      </c>
+      <c r="J1" t="str">
         <v>Food Items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1">
-        <v>45702.22928240741</v>
+        <v>45703.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>420</v>
+        <v>240</v>
       </c>
       <c r="F2">
-        <v>6.3</v>
+        <v>7.2</v>
       </c>
       <c r="G2">
-        <v>6.3</v>
+        <v>7.2</v>
       </c>
       <c r="H2">
-        <v>12.6</v>
+        <v>14.4</v>
       </c>
       <c r="I2" t="str">
-        <v>Chicken Wrap (x7)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>137</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45702.22928240741</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>152</v>
-      </c>
-      <c r="F3">
-        <v>2.2</v>
-      </c>
-      <c r="G3">
-        <v>2.2</v>
-      </c>
-      <c r="H3">
-        <v>4.4</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Mango Lassi (x1), Strawberry Lassi (x1), Butterscotch Lassi (x1)</v>
+        <v>dsf</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Chicken Schezwan Sandwich (x1), Veg Schezwan Sandwich (x1), Chicken Sandwich (x1), Veg Sandwich (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major Changes to Customers table. Add, Edit, Delete, Clear applied
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,47 +429,99 @@
         <v>Tax (₹)</v>
       </c>
       <c r="I1" t="str">
-        <v>Reason</v>
-      </c>
-      <c r="J1" t="str">
         <v>Food Items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1">
-        <v>45703.22928240741</v>
+        <v>45704.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>0.4</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>0.8</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Belgian Coffee (x1)</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>162</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45704.22928240741</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="E2">
-        <v>240</v>
-      </c>
-      <c r="F2">
-        <v>7.2</v>
-      </c>
-      <c r="G2">
-        <v>7.2</v>
-      </c>
-      <c r="H2">
-        <v>14.4</v>
-      </c>
-      <c r="I2" t="str">
-        <v>dsf</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Chicken Schezwan Sandwich (x1), Veg Schezwan Sandwich (x1), Chicken Sandwich (x1), Veg Sandwich (x1)</v>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>0.8</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>1.6</v>
+      </c>
+      <c r="I3" t="str">
+        <v>8PM Coffee (x1), Coffee Italia (x1)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>160</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45704.22928240741</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <v>2.73</v>
+      </c>
+      <c r="G4">
+        <v>2.73</v>
+      </c>
+      <c r="H4">
+        <v>5.45</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Veg Wrap (x1), Chicken Schezwan Wrap (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day End Summary refined
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,94 +434,326 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1">
-        <v>45704.22928240741</v>
+        <v>45706.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="G2">
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="H2">
-        <v>0.8</v>
+        <v>3.6</v>
       </c>
       <c r="I2" t="str">
-        <v>Belgian Coffee (x1)</v>
+        <v>Mango Lassi (x2)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="B3" s="1">
-        <v>45704.22928240741</v>
+        <v>45706.22928240741</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="F3">
-        <v>0.8</v>
+        <v>2.2</v>
       </c>
       <c r="G3">
-        <v>0.8</v>
+        <v>2.2</v>
       </c>
       <c r="H3">
-        <v>1.6</v>
+        <v>4.4</v>
       </c>
       <c r="I3" t="str">
-        <v>8PM Coffee (x1), Coffee Italia (x1)</v>
+        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
+        <v>195</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>140</v>
+      </c>
+      <c r="F4">
+        <v>1.4</v>
+      </c>
+      <c r="G4">
+        <v>1.4</v>
+      </c>
+      <c r="H4">
+        <v>2.8</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Strawberry Lassi (x1), Banana Shake (x2)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>192</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>1.3</v>
+      </c>
+      <c r="G5">
+        <v>1.3</v>
+      </c>
+      <c r="H5">
+        <v>2.6</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>191</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>160</v>
       </c>
-      <c r="B4" s="1">
-        <v>45704.22928240741</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="F6">
+        <v>2.2</v>
+      </c>
+      <c r="G6">
+        <v>2.2</v>
+      </c>
+      <c r="H6">
+        <v>4.4</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1), Chicken Wrap (x1)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>185</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>1.3</v>
+      </c>
+      <c r="G7">
+        <v>1.3</v>
+      </c>
+      <c r="H7">
+        <v>2.6</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Mango Lassi (x1), Strawberry Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>184</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
         <v>120</v>
       </c>
-      <c r="F4">
-        <v>2.73</v>
-      </c>
-      <c r="G4">
-        <v>2.73</v>
-      </c>
-      <c r="H4">
-        <v>5.45</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Veg Wrap (x1), Chicken Schezwan Wrap (x1)</v>
+      <c r="F8">
+        <v>1.8</v>
+      </c>
+      <c r="G8">
+        <v>1.8</v>
+      </c>
+      <c r="H8">
+        <v>3.6</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Butterscotch Lassi (x1), Chicken Wrap (x1)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>183</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>120</v>
+      </c>
+      <c r="F9">
+        <v>1.73</v>
+      </c>
+      <c r="G9">
+        <v>1.73</v>
+      </c>
+      <c r="H9">
+        <v>3.45</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Veg Cheese Pops (x1), Banana Shake (x1)</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>182</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>1.23</v>
+      </c>
+      <c r="G10">
+        <v>1.23</v>
+      </c>
+      <c r="H10">
+        <v>2.45</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Chicken Cheese Pops (x1)</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>181</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>1.3</v>
+      </c>
+      <c r="G11">
+        <v>1.3</v>
+      </c>
+      <c r="H11">
+        <v>2.6</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>180</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45706.22928240741</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <v>0.9</v>
+      </c>
+      <c r="G12">
+        <v>0.9</v>
+      </c>
+      <c r="H12">
+        <v>1.8</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Chicken Cheese Burger (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major changes to Categories
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,16 +434,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="B2" s="1">
-        <v>45706.22928240741</v>
+        <v>45708.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>120</v>
@@ -458,302 +458,12 @@
         <v>3.6</v>
       </c>
       <c r="I2" t="str">
-        <v>Mango Lassi (x2)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>196</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>160</v>
-      </c>
-      <c r="F3">
-        <v>2.2</v>
-      </c>
-      <c r="G3">
-        <v>2.2</v>
-      </c>
-      <c r="H3">
-        <v>4.4</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>195</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>140</v>
-      </c>
-      <c r="F4">
-        <v>1.4</v>
-      </c>
-      <c r="G4">
-        <v>1.4</v>
-      </c>
-      <c r="H4">
-        <v>2.8</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Strawberry Lassi (x1), Banana Shake (x2)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>192</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>1.3</v>
-      </c>
-      <c r="G5">
-        <v>1.3</v>
-      </c>
-      <c r="H5">
-        <v>2.6</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>191</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>160</v>
-      </c>
-      <c r="F6">
-        <v>2.2</v>
-      </c>
-      <c r="G6">
-        <v>2.2</v>
-      </c>
-      <c r="H6">
-        <v>4.4</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1), Chicken Wrap (x1)</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>185</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>1.3</v>
-      </c>
-      <c r="G7">
-        <v>1.3</v>
-      </c>
-      <c r="H7">
-        <v>2.6</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Mango Lassi (x1), Strawberry Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>184</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>120</v>
-      </c>
-      <c r="F8">
-        <v>1.8</v>
-      </c>
-      <c r="G8">
-        <v>1.8</v>
-      </c>
-      <c r="H8">
-        <v>3.6</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Butterscotch Lassi (x1), Chicken Wrap (x1)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>183</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>120</v>
-      </c>
-      <c r="F9">
-        <v>1.73</v>
-      </c>
-      <c r="G9">
-        <v>1.73</v>
-      </c>
-      <c r="H9">
-        <v>3.45</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Veg Cheese Pops (x1), Banana Shake (x1)</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>182</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>70</v>
-      </c>
-      <c r="F10">
-        <v>1.23</v>
-      </c>
-      <c r="G10">
-        <v>1.23</v>
-      </c>
-      <c r="H10">
-        <v>2.45</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Chicken Cheese Pops (x1)</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>181</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-      <c r="F11">
-        <v>1.3</v>
-      </c>
-      <c r="G11">
-        <v>1.3</v>
-      </c>
-      <c r="H11">
-        <v>2.6</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Strawberry Lassi (x1), Butterscotch Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>180</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45706.22928240741</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>60</v>
-      </c>
-      <c r="F12">
-        <v>0.9</v>
-      </c>
-      <c r="G12">
-        <v>0.9</v>
-      </c>
-      <c r="H12">
-        <v>1.8</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Chicken Cheese Burger (x1)</v>
+        <v>Butterscotch Lassi (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Export to excel functionality has been implemented for all histories
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -437,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>45723.22928240741</v>
+        <v>45841.00011574074</v>
       </c>
       <c r="D2" t="str">
         <v>₹120.00</v>
@@ -463,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>45724.22928240741</v>
+        <v>45872.00011574074</v>
       </c>
       <c r="D3" t="str">
         <v>₹180.00</v>
@@ -489,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>45724.22928240741</v>
+        <v>45872.00011574074</v>
       </c>
       <c r="D4" t="str">
         <v>₹120.00</v>
@@ -504,7 +504,7 @@
         <v>₹24.00</v>
       </c>
       <c r="H4" t="str">
-        <v>Strawberry Lassi</v>
+        <v>Strawberry Lassi, Chicken Wrap</v>
       </c>
     </row>
     <row r="5">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>45724.22928240741</v>
+        <v>45872.00011574074</v>
       </c>
       <c r="D5" t="str">
         <v>₹180.00</v>
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>45724.22928240741</v>
+        <v>45872.00011574074</v>
       </c>
       <c r="D6" t="str">
         <v>₹220.00</v>

</xml_diff>

<commit_message>
Improved the titles of all histories
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,160 +408,91 @@
         <v>Bill No</v>
       </c>
       <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Cashier</v>
+      </c>
+      <c r="D1" t="str">
         <v>KOT</v>
       </c>
-      <c r="C1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Initial Price (₹)</v>
-      </c>
       <c r="E1" t="str">
-        <v>Discount (%)</v>
+        <v>Price (₹)</v>
       </c>
       <c r="F1" t="str">
-        <v>Discount (₹)</v>
+        <v>SGST (₹)</v>
       </c>
       <c r="G1" t="str">
-        <v>Final Price (₹)</v>
+        <v>CGST (₹)</v>
       </c>
       <c r="H1" t="str">
+        <v>Tax (₹)</v>
+      </c>
+      <c r="I1" t="str">
         <v>Food Items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>405</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45841.00011574074</v>
-      </c>
-      <c r="D2" t="str">
-        <v>₹120.00</v>
+        <v>432</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45903.00011574074</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>37.5</v>
-      </c>
-      <c r="F2" t="str">
-        <v>₹45.00</v>
-      </c>
-      <c r="G2" t="str">
-        <v>₹75.00</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Vanilla Shake</v>
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>1.93</v>
+      </c>
+      <c r="G2">
+        <v>1.93</v>
+      </c>
+      <c r="H2">
+        <v>3.85</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Chicken Burger (x1), Strawberry Lassi (x1), Veg Wrap (x1)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>416</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45872.00011574074</v>
-      </c>
-      <c r="D3" t="str">
-        <v>₹180.00</v>
+        <v>433</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45903.00011574074</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="str">
-        <v>₹9.00</v>
-      </c>
-      <c r="G3" t="str">
-        <v>₹171.00</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Chicken Wrap</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>417</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45872.00011574074</v>
-      </c>
-      <c r="D4" t="str">
-        <v>₹120.00</v>
-      </c>
-      <c r="E4">
-        <v>80</v>
-      </c>
-      <c r="F4" t="str">
-        <v>₹96.00</v>
-      </c>
-      <c r="G4" t="str">
-        <v>₹24.00</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Strawberry Lassi, Chicken Wrap</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>418</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45872.00011574074</v>
-      </c>
-      <c r="D5" t="str">
-        <v>₹180.00</v>
-      </c>
-      <c r="E5">
-        <v>78</v>
-      </c>
-      <c r="F5" t="str">
-        <v>₹140.40</v>
-      </c>
-      <c r="G5" t="str">
-        <v>₹39.60</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Chicken Burger, Vanilla Shake</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>419</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45872.00011574074</v>
-      </c>
-      <c r="D6" t="str">
-        <v>₹220.00</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6" t="str">
-        <v>₹26.40</v>
-      </c>
-      <c r="G6" t="str">
-        <v>₹193.60</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Strawberry Lassi, Chicken Cheese Pops, Veg Cheese Pops</v>
+        <v>500</v>
+      </c>
+      <c r="F3">
+        <v>7.1</v>
+      </c>
+      <c r="G3">
+        <v>7.1</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Mango Lassi (x1), Strawberry Lassi (x1), Chicken Cheese Pops (x1), Veg Cheese Pops (x3)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reduced Order history and category History size in ui.js
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,65 +434,239 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>432</v>
+        <v>593</v>
       </c>
       <c r="B2" s="1">
-        <v>45903.00011574074</v>
+        <v>45692.00011574074</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="F2">
-        <v>1.93</v>
+        <v>0.9</v>
       </c>
       <c r="G2">
-        <v>1.93</v>
+        <v>0.9</v>
       </c>
       <c r="H2">
-        <v>3.85</v>
+        <v>1.8</v>
       </c>
       <c r="I2" t="str">
-        <v>Chicken Burger (x1), Strawberry Lassi (x1), Veg Wrap (x1)</v>
+        <v>Chicken Burger (x1)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>433</v>
+        <v>592</v>
       </c>
       <c r="B3" s="1">
-        <v>45903.00011574074</v>
+        <v>45692.00011574074</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>3.5</v>
+      </c>
+      <c r="G3">
+        <v>3.5</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Chicken Cheese Burger (x1), Vanilla Shake (x2), Chicken Wrap (x1)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>591</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+      <c r="H4">
+        <v>1.6</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Belgian Coffee (x2)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>590</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>500</v>
-      </c>
-      <c r="F3">
-        <v>7.1</v>
-      </c>
-      <c r="G3">
-        <v>7.1</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Mango Lassi (x1), Strawberry Lassi (x1), Chicken Cheese Pops (x1), Veg Cheese Pops (x3)</v>
+      <c r="E5">
+        <v>140</v>
+      </c>
+      <c r="F5">
+        <v>2.2</v>
+      </c>
+      <c r="G5">
+        <v>2.2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Peri Peri Fries (x2), Watermelon Juice (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>589</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>3.1</v>
+      </c>
+      <c r="G6">
+        <v>3.1</v>
+      </c>
+      <c r="H6">
+        <v>6.2</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Chicken Burger (x2), Mango Lassi (x1), Strawberry Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>588</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>180</v>
+      </c>
+      <c r="F7">
+        <v>1.2</v>
+      </c>
+      <c r="G7">
+        <v>1.2</v>
+      </c>
+      <c r="H7">
+        <v>4.2</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Vanilla Shake (x3), Chicken Cheese Burger (x1)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>587</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>370</v>
+      </c>
+      <c r="F8">
+        <v>5.03</v>
+      </c>
+      <c r="G8">
+        <v>5.03</v>
+      </c>
+      <c r="H8">
+        <v>10.05</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Oreo Shake (x1), Vanilla Shake (x1), Chicken Wrap (x2), Butterscotch Lassi (x2), Strawberry Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>586</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45692.00011574074</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+      <c r="F9">
+        <v>3.6</v>
+      </c>
+      <c r="G9">
+        <v>3.6</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Chicken Burger (x2), Chicken Cheese Burger (x1), Butterscotch Lassi (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replace most alerts and exit dialog. However, still need work on export to excel
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -64,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,16 +433,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>593</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45692.00011574074</v>
+        <v>675</v>
+      </c>
+      <c r="B2" t="str">
+        <v>20-04-25</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>60</v>
@@ -458,215 +457,12 @@
         <v>1.8</v>
       </c>
       <c r="I2" t="str">
-        <v>Chicken Burger (x1)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>592</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="F3">
-        <v>3.5</v>
-      </c>
-      <c r="G3">
-        <v>3.5</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Chicken Cheese Burger (x1), Vanilla Shake (x2), Chicken Wrap (x1)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>591</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <v>0.8</v>
-      </c>
-      <c r="G4">
-        <v>0.8</v>
-      </c>
-      <c r="H4">
-        <v>1.6</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Belgian Coffee (x2)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>590</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>140</v>
-      </c>
-      <c r="F5">
-        <v>2.2</v>
-      </c>
-      <c r="G5">
-        <v>2.2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Peri Peri Fries (x2), Watermelon Juice (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>589</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>220</v>
-      </c>
-      <c r="F6">
-        <v>3.1</v>
-      </c>
-      <c r="G6">
-        <v>3.1</v>
-      </c>
-      <c r="H6">
-        <v>6.2</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Chicken Burger (x2), Mango Lassi (x1), Strawberry Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>588</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>180</v>
-      </c>
-      <c r="F7">
-        <v>1.2</v>
-      </c>
-      <c r="G7">
-        <v>1.2</v>
-      </c>
-      <c r="H7">
-        <v>4.2</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Vanilla Shake (x3), Chicken Cheese Burger (x1)</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>587</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>370</v>
-      </c>
-      <c r="F8">
-        <v>5.03</v>
-      </c>
-      <c r="G8">
-        <v>5.03</v>
-      </c>
-      <c r="H8">
-        <v>10.05</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Oreo Shake (x1), Vanilla Shake (x1), Chicken Wrap (x2), Butterscotch Lassi (x2), Strawberry Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>586</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45692.00011574074</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>3.6</v>
-      </c>
-      <c r="G9">
-        <v>3.6</v>
-      </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Chicken Burger (x2), Chicken Cheese Burger (x1), Butterscotch Lassi (x2)</v>
+        <v>Chicken Wrap (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>